<commit_message>
modified tests, some error corrections
Former-commit-id: 416ae47e02208b26eb1fa6d34e09f4b014204106
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_tax_sched.xlsx
+++ b/tests/test_data/test_dfs_tax_sched.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>tu_id</t>
   </si>
@@ -47,6 +47,27 @@
   </si>
   <si>
     <t>gross_e5</t>
+  </si>
+  <si>
+    <t>tax_kfb</t>
+  </si>
+  <si>
+    <t>abgst</t>
+  </si>
+  <si>
+    <t>abgst_tu</t>
+  </si>
+  <si>
+    <t>tax_abg_kfb</t>
+  </si>
+  <si>
+    <t>tax_abg_nokfb</t>
+  </si>
+  <si>
+    <t>zve_abg_nokfb</t>
+  </si>
+  <si>
+    <t>zve_abg_kfb</t>
   </si>
 </sst>
 </file>
@@ -396,20 +417,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="1"/>
+    <col min="10" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -423,29 +446,50 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="S1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="X1"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -457,34 +501,59 @@
         <v>5000</v>
       </c>
       <c r="D2">
-        <f>C2</f>
         <v>5000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>5500</v>
       </c>
       <c r="F2">
+        <v>5500</v>
+      </c>
+      <c r="G2">
+        <v>500</v>
+      </c>
+      <c r="H2">
         <v>2018</v>
       </c>
-      <c r="H2" s="2">
+      <c r="J2" s="2">
         <f>TRUNC((C2&gt;9000)*(C2&lt;13996)*(997.8*(C2-9000)/10000+1400)*(C2-9000)/10000+(C2&gt;13996)*(C2&lt;54949)*((220.13*(C2-13996)/10000+2397)*(C2-13996)/10000+948.49)+(C2&gt;54950)*(C2&lt;260532)*(0.42*C2-8621.75)+(C2&gt;260532)*(0.45*C2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
+        <f>TRUNC((D2&gt;9000)*(D2&lt;13996)*(997.8*(D2-9000)/10000+1400)*(D2-9000)/10000+(D2&gt;13996)*(D2&lt;54949)*((220.13*(D2-13996)/10000+2397)*(D2-13996)/10000+948.49)+(D2&gt;54950)*(D2&lt;260532)*(0.42*D2-8621.75)+(D2&gt;260532)*(0.45*D2-16437.7))</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <f>TRUNC((E2&gt;9000)*(E2&lt;13996)*(997.8*(E2-9000)/10000+1400)*(E2-9000)/10000+(E2&gt;13996)*(E2&lt;54949)*((220.13*(E2-13996)/10000+2397)*(E2-13996)/10000+948.49)+(E2&gt;54950)*(E2&lt;260532)*(0.42*E2-8621.75)+(E2&gt;260532)*(0.45*E2-16437.7))</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <f>TRUNC((F2&gt;9000)*(F2&lt;13996)*(997.8*(F2-9000)/10000+1400)*(F2-9000)/10000+(F2&gt;13996)*(F2&lt;54949)*((220.13*(F2-13996)/10000+2397)*(F2-13996)/10000+948.49)+(F2&gt;54950)*(F2&lt;260532)*(0.42*F2-8621.75)+(F2&gt;260532)*(0.45*F2-16437.7))</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>MAX((G2-801)*0.25,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>N2</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>9000</v>
       </c>
-      <c r="L2">
+      <c r="Q2">
         <v>13996</v>
       </c>
-      <c r="M2">
+      <c r="R2">
         <v>54949</v>
       </c>
-      <c r="N2">
+      <c r="S2">
         <v>260532</v>
       </c>
-      <c r="S2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="X2"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A6" si="0">B3</f>
         <v>2</v>
@@ -496,34 +565,60 @@
         <v>10000</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="1">C3</f>
+        <f t="shared" ref="D3:D4" si="1">C3</f>
         <v>10000</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="F3">
+        <v>12000</v>
+      </c>
+      <c r="G3">
+        <v>2000</v>
+      </c>
+      <c r="H3">
         <v>2015</v>
       </c>
-      <c r="H3" s="2">
-        <f>TRUNC((C3&gt;K3)*(C3&lt;L3)*(974.58*(C3-K3)/10000+1400)*(C3-K3)/10000+(C3&gt;L3)*(C3&lt;M3)*((228.74*(C3-L3)/10000+2397)*(C3-L3)/10000+971)+(C3&gt;M3)*(C3&lt;N3)*(0.42*C3-8237)+(C3&gt;N3)*(0.45*C3-15761))</f>
+      <c r="J3" s="2">
+        <f>TRUNC((C3&gt;P3)*(C3&lt;Q3)*(974.58*(C3-P3)/10000+1400)*(C3-P3)/10000+(C3&gt;Q3)*(C3&lt;R3)*((228.74*(C3-Q3)/10000+2397)*(C3-Q3)/10000+971)+(C3&gt;R3)*(C3&lt;S3)*(0.42*C3-8239)+(C3&gt;S3)*(0.45*C3-15761))</f>
         <v>236</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
+        <f>TRUNC((D3&gt;P3)*(D3&lt;Q3)*(974.58*(D3-P3)/10000+1400)*(D3-P3)/10000+(D3&gt;Q3)*(D3&lt;R3)*((228.74*(D3-Q3)/10000+2397)*(D3-Q3)/10000+971)+(D3&gt;R3)*(D3&lt;S3)*(0.42*D3-8239)+(D3&gt;S3)*(0.45*D3-15761))</f>
+        <v>236</v>
+      </c>
+      <c r="L3" s="2">
+        <f>TRUNC((E3&gt;P3)*(E3&lt;Q3)*(974.58*(E3-P3)/10000+1400)*(E3-P3)/10000+(E3&gt;Q3)*(E3&lt;R3)*((228.74*(E3-Q3)/10000+2397)*(E3-Q3)/10000+971)+(E3&gt;R3)*(E3&lt;S3)*(0.42*E3-8239)+(E3&gt;S3)*(0.45*E3-15761))</f>
+        <v>615</v>
+      </c>
+      <c r="M3" s="2">
+        <f>TRUNC((F3&gt;P3)*(F3&lt;Q3)*(974.58*(F3-P3)/10000+1400)*(F3-P3)/10000+(F3&gt;Q3)*(F3&lt;S3)*((228.74*(F3-Q3)/10000+2397)*(F3-R3)/10000+971)+(F3&gt;S3)*(F3&lt;S3)*(0.42*F3-8239)+(F3&gt;S3)*(0.45*F3-15761))</f>
+        <v>615</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N6" si="2">MAX((G3-801)*0.25,0)</f>
+        <v>299.75</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O6" si="3">N3</f>
+        <v>299.75</v>
+      </c>
+      <c r="P3">
         <v>8472</v>
       </c>
-      <c r="L3">
+      <c r="Q3">
         <v>13469</v>
       </c>
-      <c r="M3">
+      <c r="R3">
         <v>52881</v>
       </c>
-      <c r="N3">
+      <c r="S3">
         <v>250730</v>
       </c>
-      <c r="S3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="X3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -539,30 +634,56 @@
         <v>20000</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>21000</v>
       </c>
       <c r="F4">
+        <v>21000</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
         <v>2012</v>
       </c>
-      <c r="H4" s="2">
-        <f>TRUNC((C4&gt;K4)*(C4&lt;L4)*(974.58*(C4-K4)/10000+1400)*(C4-K4)/10000+(C4&gt;L4)*(C4&lt;M4)*((228.74*(C4-L4)/10000+2397)*(C4-L4)/10000+1038)+(C4&gt;M4)*(C4&lt;N4)*(0.42*C4-8172)+(C4&gt;N4)*(0.45*C4-15694))</f>
-        <v>2701</v>
-      </c>
-      <c r="K4">
+      <c r="J4" s="2">
+        <f>TRUNC((C4&gt;P4)*(C4&lt;Q4)*(939.68*(C4-P4)/10000+1400)*(C4-P4)/10000+(C4&gt;Q4)*(C4&lt;R4)*((228.74*(C4-Q4)/10000+2397)*(C4-Q4)/10000+1007)+(C4&gt;R4)*(C4&lt;S4)*(0.42*C4-8064)+(C4&gt;S4)*(0.45*C4-15576))</f>
+        <v>2670</v>
+      </c>
+      <c r="K4" s="2">
+        <f>TRUNC((D4&gt;P4)*(D4&lt;Q4)*(939.68*(D4-P4)/10000+1400)*(D4-P4)/10000+(D4&gt;Q4)*(D4&lt;R4)*((228.74*(D4-Q4)/10000+2397)*(D4-Q4)/10000+1007)+(D4&gt;R4)*(D4&lt;S4)*(0.42*D4-8064)+(D4&gt;S4)*(0.45*D4-15576))</f>
+        <v>2670</v>
+      </c>
+      <c r="L4" s="2">
+        <f>TRUNC((E4&gt;P4)*(E4&lt;Q4)*(939.68*(E4-P4)/10000+1400)*(E4-P4)/10000+(E4&gt;Q4)*(E4&lt;R4)*((228.74*(E4-Q4)/10000+2397)*(E4-Q4)/10000+1007)+(E4&gt;R4)*(E4&lt;S4)*(0.42*E4-8064)+(E4&gt;S4)*(0.45*E4-15576))</f>
+        <v>2941</v>
+      </c>
+      <c r="M4" s="2">
+        <f>TRUNC((F4&gt;P4)*(F4&lt;Q4)*(939.68*(F4-P4)/10000+1400)*(F4-P4)/10000+(F4&gt;Q4)*(F4&lt;R4)*((228.74*(F4-Q4)/10000+2397)*(F4-Q4)/10000+1007)+(F4&gt;R4)*(F4&lt;S4)*(0.42*F4-8064)+(F4&gt;S4)*(0.45*F4-15576))</f>
+        <v>2941</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>49.75</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="3"/>
+        <v>49.75</v>
+      </c>
+      <c r="P4">
         <v>8004</v>
       </c>
-      <c r="L4">
+      <c r="Q4">
         <v>13469</v>
       </c>
-      <c r="M4">
+      <c r="R4">
         <v>52881</v>
       </c>
-      <c r="N4">
+      <c r="S4">
         <v>250730</v>
       </c>
-      <c r="S4"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="X4"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -574,34 +695,59 @@
         <v>50000</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>42000</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>52500</v>
       </c>
       <c r="F5">
+        <v>44500</v>
+      </c>
+      <c r="G5">
+        <v>2500</v>
+      </c>
+      <c r="H5">
         <v>2009</v>
       </c>
-      <c r="H5" s="2">
-        <f>TRUNC((C5&gt;K5)*(C5&lt;L5)*(883.74*(C5-K5)/10000+1500)*(C5-K5)/10000+(C5&gt;L5)*(C5&lt;M5)*((228.74*(C5-L5)/10000+2397)*(C5-L5)/10000+989)+(C5&gt;M5)*(C5&lt;N5)*(0.42*C5-7914)+(C5&gt;N5)*(0.45*C5-15414))</f>
+      <c r="J5" s="2">
+        <f>TRUNC((C5&gt;P5)*(C5&lt;Q5)*(883.74*(C5-P5)/10000+1500)*(C5-P5)/10000+(C5&gt;Q5)*(C5&lt;R5)*((228.74*(C5-Q5)/10000+2397)*(C5-Q5)/10000+989)+(C5&gt;R5)*(C5&lt;S5)*(0.42*C5-7914)+(C5&gt;S5)*(0.45*C5-15414))</f>
         <v>13096</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
+        <f>TRUNC((D5&gt;P5)*(D5&lt;Q5)*(883.74*(D5-P5)/10000+1500)*(D5-P5)/10000+(D5&gt;Q5)*(D5&lt;R5)*((228.74*(D5-Q5)/10000+2397)*(D5-Q5)/10000+989)+(D5&gt;R5)*(D5&lt;S5)*(0.42*D5-7914)+(D5&gt;S5)*(0.45*D5-15414))</f>
+        <v>9961</v>
+      </c>
+      <c r="L5" s="2">
+        <f>TRUNC((E5&gt;P5)*(E5&lt;Q5)*(883.74*(E5-P5)/10000+1500)*(E5-P5)/10000+(E5&gt;Q5)*(E5&lt;R5)*((228.74*(E5-Q5)/10000+2397)*(E5-Q5)/10000+989)+(E5&gt;R5)*(E5&lt;S5)*(0.42*E5-7914)+(E5&gt;S5)*(0.45*E5-15414))</f>
+        <v>14136</v>
+      </c>
+      <c r="M5" s="2">
+        <f>TRUNC((F5&gt;P5)*(F5&lt;Q5)*(883.74*(F5-P5)/10000+1500)*(F5-P5)/10000+(F5&gt;Q5)*(F5&lt;R5)*((228.74*(F5-Q5)/10000+2397)*(F5-Q5)/10000+989)+(F5&gt;R5)*(F5&lt;S5)*(0.42*F5-7914)+(F5&gt;S5)*(0.45*F5-15414))</f>
+        <v>10909</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>424.75</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>424.75</v>
+      </c>
+      <c r="P5">
         <v>7664</v>
       </c>
-      <c r="L5">
+      <c r="Q5">
         <v>12739</v>
       </c>
-      <c r="M5">
+      <c r="R5">
         <v>52152</v>
       </c>
-      <c r="N5">
+      <c r="S5">
         <v>250000</v>
       </c>
-      <c r="S5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="X5"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -613,83 +759,108 @@
         <v>200000</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <v>180000</v>
+      </c>
+      <c r="E6">
         <v>200000</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
+        <v>180000</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>2018</v>
       </c>
-      <c r="H6" s="2">
+      <c r="J6" s="2">
         <f>TRUNC((C6&gt;9000)*(C6&lt;13996)*(997.8*(C6-9000)/10000+1400)*(C6-9000)/10000+(C6&gt;13996)*(C6&lt;54949)*((220.13*(C6-13996)/10000+2397)*(C6-13996)/10000+948.49)+(C6&gt;54950)*(C6&lt;260532)*(0.42*C6-8621.75)+(C6&gt;260532)*(0.45*C6-16437.7))</f>
         <v>75378</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
+        <f>TRUNC((D6&gt;9000)*(D6&lt;13996)*(997.8*(D6-9000)/10000+1400)*(D6-9000)/10000+(D6&gt;13996)*(D6&lt;54949)*((220.13*(D6-13996)/10000+2397)*(D6-13996)/10000+948.49)+(D6&gt;54950)*(D6&lt;260532)*(0.42*D6-8621.75)+(D6&gt;260532)*(0.45*D6-16437.7))</f>
+        <v>66978</v>
+      </c>
+      <c r="L6" s="2">
+        <f>TRUNC((E6&gt;9000)*(E6&lt;13996)*(997.8*(E6-9000)/10000+1400)*(E6-9000)/10000+(E6&gt;13996)*(E6&lt;54949)*((220.13*(E6-13996)/10000+2397)*(E6-13996)/10000+948.49)+(E6&gt;54950)*(E6&lt;260532)*(0.42*E6-8621.75)+(E6&gt;260532)*(0.45*E6-16437.7))</f>
+        <v>75378</v>
+      </c>
+      <c r="M6" s="2">
+        <f>TRUNC((F6&gt;9000)*(F6&lt;13996)*(997.8*(F6-9000)/10000+1400)*(F6-9000)/10000+(F6&gt;13996)*(F6&lt;54949)*((220.13*(F6-13996)/10000+2397)*(F6-13996)/10000+948.49)+(F6&gt;54950)*(F6&lt;260532)*(0.42*F6-8621.75)+(F6&gt;260532)*(0.45*F6-16437.7))</f>
+        <v>66978</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>9000</v>
       </c>
-      <c r="L6">
+      <c r="Q6">
         <v>13996</v>
       </c>
-      <c r="M6">
+      <c r="R6">
         <v>54949</v>
       </c>
-      <c r="N6">
+      <c r="S6">
         <v>260532</v>
       </c>
-      <c r="S6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S17" s="2"/>
-    </row>
-    <row r="18" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="2"/>
-    </row>
-    <row r="19" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S19" s="2"/>
-    </row>
-    <row r="20" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S20" s="2"/>
-    </row>
-    <row r="21" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S21" s="2"/>
-    </row>
-    <row r="22" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S22" s="2"/>
-    </row>
-    <row r="23" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S23" s="2"/>
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X7" s="2"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X9" s="2"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X10" s="2"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X11" s="2"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X15" s="2"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X16" s="2"/>
+    </row>
+    <row r="17" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tax schedule test correction
Former-commit-id: 3a91dbf64ecbd1d1dff90437145934c4d97528fe
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_tax_sched.xlsx
+++ b/tests/test_data/test_dfs_tax_sched.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>tu_id</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>zve_abg_kfb</t>
+  </si>
+  <si>
+    <t>zveranl</t>
   </si>
 </sst>
 </file>
@@ -417,22 +420,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="1"/>
+    <col min="11" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -455,41 +458,44 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>9</v>
       </c>
-      <c r="X1"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -512,48 +518,51 @@
       <c r="G2">
         <v>500</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>2018</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <f>TRUNC((C2&gt;9000)*(C2&lt;13996)*(997.8*(C2-9000)/10000+1400)*(C2-9000)/10000+(C2&gt;13996)*(C2&lt;54949)*((220.13*(C2-13996)/10000+2397)*(C2-13996)/10000+948.49)+(C2&gt;54950)*(C2&lt;260532)*(0.42*C2-8621.75)+(C2&gt;260532)*(0.45*C2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <f>TRUNC((D2&gt;9000)*(D2&lt;13996)*(997.8*(D2-9000)/10000+1400)*(D2-9000)/10000+(D2&gt;13996)*(D2&lt;54949)*((220.13*(D2-13996)/10000+2397)*(D2-13996)/10000+948.49)+(D2&gt;54950)*(D2&lt;260532)*(0.42*D2-8621.75)+(D2&gt;260532)*(0.45*D2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <f>TRUNC((E2&gt;9000)*(E2&lt;13996)*(997.8*(E2-9000)/10000+1400)*(E2-9000)/10000+(E2&gt;13996)*(E2&lt;54949)*((220.13*(E2-13996)/10000+2397)*(E2-13996)/10000+948.49)+(E2&gt;54950)*(E2&lt;260532)*(0.42*E2-8621.75)+(E2&gt;260532)*(0.45*E2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <f>TRUNC((F2&gt;9000)*(F2&lt;13996)*(997.8*(F2-9000)/10000+1400)*(F2-9000)/10000+(F2&gt;13996)*(F2&lt;54949)*((220.13*(F2-13996)/10000+2397)*(F2-13996)/10000+948.49)+(F2&gt;54950)*(F2&lt;260532)*(0.42*F2-8621.75)+(F2&gt;260532)*(0.45*F2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <f>MAX((G2-801)*0.25,0)</f>
         <v>0</v>
       </c>
-      <c r="O2">
-        <f>N2</f>
-        <v>0</v>
-      </c>
       <c r="P2">
+        <f>O2</f>
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>9000</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>13996</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>54949</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>260532</v>
       </c>
-      <c r="X2"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A6" si="0">B3</f>
         <v>2</v>
@@ -577,48 +586,51 @@
       <c r="G3">
         <v>2000</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>2015</v>
       </c>
-      <c r="J3" s="2">
-        <f>TRUNC((C3&gt;P3)*(C3&lt;Q3)*(974.58*(C3-P3)/10000+1400)*(C3-P3)/10000+(C3&gt;Q3)*(C3&lt;R3)*((228.74*(C3-Q3)/10000+2397)*(C3-Q3)/10000+971)+(C3&gt;R3)*(C3&lt;S3)*(0.42*C3-8239)+(C3&gt;S3)*(0.45*C3-15761))</f>
+      <c r="K3" s="2">
+        <f>TRUNC((C3&gt;Q3)*(C3&lt;R3)*(974.58*(C3-Q3)/10000+1400)*(C3-Q3)/10000+(C3&gt;R3)*(C3&lt;S3)*((228.74*(C3-R3)/10000+2397)*(C3-R3)/10000+971)+(C3&gt;S3)*(C3&lt;T3)*(0.42*C3-8239)+(C3&gt;T3)*(0.45*C3-15761))</f>
         <v>236</v>
       </c>
-      <c r="K3" s="2">
-        <f>TRUNC((D3&gt;P3)*(D3&lt;Q3)*(974.58*(D3-P3)/10000+1400)*(D3-P3)/10000+(D3&gt;Q3)*(D3&lt;R3)*((228.74*(D3-Q3)/10000+2397)*(D3-Q3)/10000+971)+(D3&gt;R3)*(D3&lt;S3)*(0.42*D3-8239)+(D3&gt;S3)*(0.45*D3-15761))</f>
+      <c r="L3" s="2">
+        <f>TRUNC((D3&gt;Q3)*(D3&lt;R3)*(974.58*(D3-Q3)/10000+1400)*(D3-Q3)/10000+(D3&gt;R3)*(D3&lt;S3)*((228.74*(D3-R3)/10000+2397)*(D3-R3)/10000+971)+(D3&gt;S3)*(D3&lt;T3)*(0.42*D3-8239)+(D3&gt;T3)*(0.45*D3-15761))</f>
         <v>236</v>
       </c>
-      <c r="L3" s="2">
-        <f>TRUNC((E3&gt;P3)*(E3&lt;Q3)*(974.58*(E3-P3)/10000+1400)*(E3-P3)/10000+(E3&gt;Q3)*(E3&lt;R3)*((228.74*(E3-Q3)/10000+2397)*(E3-Q3)/10000+971)+(E3&gt;R3)*(E3&lt;S3)*(0.42*E3-8239)+(E3&gt;S3)*(0.45*E3-15761))</f>
+      <c r="M3" s="2">
+        <f>TRUNC((E3&gt;Q3)*(E3&lt;R3)*(974.58*(E3-Q3)/10000+1400)*(E3-Q3)/10000+(E3&gt;R3)*(E3&lt;S3)*((228.74*(E3-R3)/10000+2397)*(E3-R3)/10000+971)+(E3&gt;S3)*(E3&lt;T3)*(0.42*E3-8239)+(E3&gt;T3)*(0.45*E3-15761))</f>
         <v>615</v>
       </c>
-      <c r="M3" s="2">
-        <f>TRUNC((F3&gt;P3)*(F3&lt;Q3)*(974.58*(F3-P3)/10000+1400)*(F3-P3)/10000+(F3&gt;Q3)*(F3&lt;S3)*((228.74*(F3-Q3)/10000+2397)*(F3-R3)/10000+971)+(F3&gt;S3)*(F3&lt;S3)*(0.42*F3-8239)+(F3&gt;S3)*(0.45*F3-15761))</f>
+      <c r="N3" s="2">
+        <f>TRUNC((F3&gt;Q3)*(F3&lt;R3)*(974.58*(F3-Q3)/10000+1400)*(F3-Q3)/10000+(F3&gt;R3)*(F3&lt;T3)*((228.74*(F3-R3)/10000+2397)*(F3-S3)/10000+971)+(F3&gt;T3)*(F3&lt;T3)*(0.42*F3-8239)+(F3&gt;T3)*(0.45*F3-15761))</f>
         <v>615</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N6" si="2">MAX((G3-801)*0.25,0)</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O6" si="2">MAX((G3-801)*0.25,0)</f>
         <v>299.75</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O6" si="3">N3</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P6" si="3">O3</f>
         <v>299.75</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>8472</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>13469</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>52881</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>250730</v>
       </c>
-      <c r="X3"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -642,48 +654,51 @@
       <c r="G4">
         <v>1000</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>2012</v>
       </c>
-      <c r="J4" s="2">
-        <f>TRUNC((C4&gt;P4)*(C4&lt;Q4)*(939.68*(C4-P4)/10000+1400)*(C4-P4)/10000+(C4&gt;Q4)*(C4&lt;R4)*((228.74*(C4-Q4)/10000+2397)*(C4-Q4)/10000+1007)+(C4&gt;R4)*(C4&lt;S4)*(0.42*C4-8064)+(C4&gt;S4)*(0.45*C4-15576))</f>
+      <c r="K4" s="2">
+        <f>TRUNC((C4&gt;Q4)*(C4&lt;R4)*(939.68*(C4-Q4)/10000+1400)*(C4-Q4)/10000+(C4&gt;R4)*(C4&lt;S4)*((228.74*(C4-R4)/10000+2397)*(C4-R4)/10000+1007)+(C4&gt;S4)*(C4&lt;T4)*(0.42*C4-8064)+(C4&gt;T4)*(0.45*C4-15576))</f>
         <v>2670</v>
       </c>
-      <c r="K4" s="2">
-        <f>TRUNC((D4&gt;P4)*(D4&lt;Q4)*(939.68*(D4-P4)/10000+1400)*(D4-P4)/10000+(D4&gt;Q4)*(D4&lt;R4)*((228.74*(D4-Q4)/10000+2397)*(D4-Q4)/10000+1007)+(D4&gt;R4)*(D4&lt;S4)*(0.42*D4-8064)+(D4&gt;S4)*(0.45*D4-15576))</f>
+      <c r="L4" s="2">
+        <f>TRUNC((D4&gt;Q4)*(D4&lt;R4)*(939.68*(D4-Q4)/10000+1400)*(D4-Q4)/10000+(D4&gt;R4)*(D4&lt;S4)*((228.74*(D4-R4)/10000+2397)*(D4-R4)/10000+1007)+(D4&gt;S4)*(D4&lt;T4)*(0.42*D4-8064)+(D4&gt;T4)*(0.45*D4-15576))</f>
         <v>2670</v>
       </c>
-      <c r="L4" s="2">
-        <f>TRUNC((E4&gt;P4)*(E4&lt;Q4)*(939.68*(E4-P4)/10000+1400)*(E4-P4)/10000+(E4&gt;Q4)*(E4&lt;R4)*((228.74*(E4-Q4)/10000+2397)*(E4-Q4)/10000+1007)+(E4&gt;R4)*(E4&lt;S4)*(0.42*E4-8064)+(E4&gt;S4)*(0.45*E4-15576))</f>
+      <c r="M4" s="2">
+        <f>TRUNC((E4&gt;Q4)*(E4&lt;R4)*(939.68*(E4-Q4)/10000+1400)*(E4-Q4)/10000+(E4&gt;R4)*(E4&lt;S4)*((228.74*(E4-R4)/10000+2397)*(E4-R4)/10000+1007)+(E4&gt;S4)*(E4&lt;T4)*(0.42*E4-8064)+(E4&gt;T4)*(0.45*E4-15576))</f>
         <v>2941</v>
       </c>
-      <c r="M4" s="2">
-        <f>TRUNC((F4&gt;P4)*(F4&lt;Q4)*(939.68*(F4-P4)/10000+1400)*(F4-P4)/10000+(F4&gt;Q4)*(F4&lt;R4)*((228.74*(F4-Q4)/10000+2397)*(F4-Q4)/10000+1007)+(F4&gt;R4)*(F4&lt;S4)*(0.42*F4-8064)+(F4&gt;S4)*(0.45*F4-15576))</f>
+      <c r="N4" s="2">
+        <f>TRUNC((F4&gt;Q4)*(F4&lt;R4)*(939.68*(F4-Q4)/10000+1400)*(F4-Q4)/10000+(F4&gt;R4)*(F4&lt;S4)*((228.74*(F4-R4)/10000+2397)*(F4-R4)/10000+1007)+(F4&gt;S4)*(F4&lt;T4)*(0.42*F4-8064)+(F4&gt;T4)*(0.45*F4-15576))</f>
         <v>2941</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <f t="shared" si="2"/>
         <v>49.75</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f t="shared" si="3"/>
         <v>49.75</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>8004</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>13469</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>52881</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>250730</v>
       </c>
-      <c r="X4"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -706,48 +721,51 @@
       <c r="G5">
         <v>2500</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>2009</v>
       </c>
-      <c r="J5" s="2">
-        <f>TRUNC((C5&gt;P5)*(C5&lt;Q5)*(883.74*(C5-P5)/10000+1500)*(C5-P5)/10000+(C5&gt;Q5)*(C5&lt;R5)*((228.74*(C5-Q5)/10000+2397)*(C5-Q5)/10000+989)+(C5&gt;R5)*(C5&lt;S5)*(0.42*C5-7914)+(C5&gt;S5)*(0.45*C5-15414))</f>
+      <c r="K5" s="2">
+        <f>TRUNC((C5&gt;Q5)*(C5&lt;R5)*(883.74*(C5-Q5)/10000+1500)*(C5-Q5)/10000+(C5&gt;R5)*(C5&lt;S5)*((228.74*(C5-R5)/10000+2397)*(C5-R5)/10000+989)+(C5&gt;S5)*(C5&lt;T5)*(0.42*C5-7914)+(C5&gt;T5)*(0.45*C5-15414))</f>
         <v>13096</v>
       </c>
-      <c r="K5" s="2">
-        <f>TRUNC((D5&gt;P5)*(D5&lt;Q5)*(883.74*(D5-P5)/10000+1500)*(D5-P5)/10000+(D5&gt;Q5)*(D5&lt;R5)*((228.74*(D5-Q5)/10000+2397)*(D5-Q5)/10000+989)+(D5&gt;R5)*(D5&lt;S5)*(0.42*D5-7914)+(D5&gt;S5)*(0.45*D5-15414))</f>
+      <c r="L5" s="2">
+        <f>TRUNC((D5&gt;Q5)*(D5&lt;R5)*(883.74*(D5-Q5)/10000+1500)*(D5-Q5)/10000+(D5&gt;R5)*(D5&lt;S5)*((228.74*(D5-R5)/10000+2397)*(D5-R5)/10000+989)+(D5&gt;S5)*(D5&lt;T5)*(0.42*D5-7914)+(D5&gt;T5)*(0.45*D5-15414))</f>
         <v>9961</v>
       </c>
-      <c r="L5" s="2">
-        <f>TRUNC((E5&gt;P5)*(E5&lt;Q5)*(883.74*(E5-P5)/10000+1500)*(E5-P5)/10000+(E5&gt;Q5)*(E5&lt;R5)*((228.74*(E5-Q5)/10000+2397)*(E5-Q5)/10000+989)+(E5&gt;R5)*(E5&lt;S5)*(0.42*E5-7914)+(E5&gt;S5)*(0.45*E5-15414))</f>
+      <c r="M5" s="2">
+        <f>TRUNC((E5&gt;Q5)*(E5&lt;R5)*(883.74*(E5-Q5)/10000+1500)*(E5-Q5)/10000+(E5&gt;R5)*(E5&lt;S5)*((228.74*(E5-R5)/10000+2397)*(E5-R5)/10000+989)+(E5&gt;S5)*(E5&lt;T5)*(0.42*E5-7914)+(E5&gt;T5)*(0.45*E5-15414))</f>
         <v>14136</v>
       </c>
-      <c r="M5" s="2">
-        <f>TRUNC((F5&gt;P5)*(F5&lt;Q5)*(883.74*(F5-P5)/10000+1500)*(F5-P5)/10000+(F5&gt;Q5)*(F5&lt;R5)*((228.74*(F5-Q5)/10000+2397)*(F5-Q5)/10000+989)+(F5&gt;R5)*(F5&lt;S5)*(0.42*F5-7914)+(F5&gt;S5)*(0.45*F5-15414))</f>
+      <c r="N5" s="2">
+        <f>TRUNC((F5&gt;Q5)*(F5&lt;R5)*(883.74*(F5-Q5)/10000+1500)*(F5-Q5)/10000+(F5&gt;R5)*(F5&lt;S5)*((228.74*(F5-R5)/10000+2397)*(F5-R5)/10000+989)+(F5&gt;S5)*(F5&lt;T5)*(0.42*F5-7914)+(F5&gt;T5)*(0.45*F5-15414))</f>
         <v>10909</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f t="shared" si="2"/>
         <v>424.75</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f t="shared" si="3"/>
         <v>424.75</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>7664</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>12739</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>52152</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>250000</v>
       </c>
-      <c r="X5"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -770,97 +788,100 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>2018</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <f>TRUNC((C6&gt;9000)*(C6&lt;13996)*(997.8*(C6-9000)/10000+1400)*(C6-9000)/10000+(C6&gt;13996)*(C6&lt;54949)*((220.13*(C6-13996)/10000+2397)*(C6-13996)/10000+948.49)+(C6&gt;54950)*(C6&lt;260532)*(0.42*C6-8621.75)+(C6&gt;260532)*(0.45*C6-16437.7))</f>
         <v>75378</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <f>TRUNC((D6&gt;9000)*(D6&lt;13996)*(997.8*(D6-9000)/10000+1400)*(D6-9000)/10000+(D6&gt;13996)*(D6&lt;54949)*((220.13*(D6-13996)/10000+2397)*(D6-13996)/10000+948.49)+(D6&gt;54950)*(D6&lt;260532)*(0.42*D6-8621.75)+(D6&gt;260532)*(0.45*D6-16437.7))</f>
         <v>66978</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <f>TRUNC((E6&gt;9000)*(E6&lt;13996)*(997.8*(E6-9000)/10000+1400)*(E6-9000)/10000+(E6&gt;13996)*(E6&lt;54949)*((220.13*(E6-13996)/10000+2397)*(E6-13996)/10000+948.49)+(E6&gt;54950)*(E6&lt;260532)*(0.42*E6-8621.75)+(E6&gt;260532)*(0.45*E6-16437.7))</f>
         <v>75378</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <f>TRUNC((F6&gt;9000)*(F6&lt;13996)*(997.8*(F6-9000)/10000+1400)*(F6-9000)/10000+(F6&gt;13996)*(F6&lt;54949)*((220.13*(F6-13996)/10000+2397)*(F6-13996)/10000+948.49)+(F6&gt;54950)*(F6&lt;260532)*(0.42*F6-8621.75)+(F6&gt;260532)*(0.45*F6-16437.7))</f>
         <v>66978</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>9000</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>13996</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>54949</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>260532</v>
       </c>
-      <c r="X6"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X7" s="2"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X9" s="2"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X10" s="2"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X11" s="2"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X12" s="2"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X13" s="2"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X14" s="2"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X15" s="2"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X16" s="2"/>
-    </row>
-    <row r="17" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X17" s="2"/>
-    </row>
-    <row r="18" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X18" s="2"/>
-    </row>
-    <row r="19" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X19" s="2"/>
-    </row>
-    <row r="20" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X20" s="2"/>
-    </row>
-    <row r="21" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X21" s="2"/>
-    </row>
-    <row r="22" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X22" s="2"/>
-    </row>
-    <row r="23" spans="24:24" x14ac:dyDescent="0.25">
-      <c r="X23" s="2"/>
+      <c r="Y6"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y9" s="2"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y10" s="2"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y12" s="2"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y14" s="2"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y16" s="2"/>
+    </row>
+    <row r="17" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y17" s="2"/>
+    </row>
+    <row r="18" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y19" s="2"/>
+    </row>
+    <row r="20" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y22" s="2"/>
+    </row>
+    <row r="23" spans="25:25" x14ac:dyDescent="0.25">
+      <c r="Y23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tax sched test correction #2
Former-commit-id: 6d4917c4391b148b204808d1314a6fed78191b9b
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_tax_sched.xlsx
+++ b/tests/test_data/test_dfs_tax_sched.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>tu_id</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>zveranl</t>
+  </si>
+  <si>
+    <t>gross_e5_tu</t>
   </si>
 </sst>
 </file>
@@ -420,22 +423,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="1"/>
+    <col min="12" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -458,44 +461,47 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>9</v>
       </c>
-      <c r="Y1"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -518,51 +524,54 @@
       <c r="G2">
         <v>500</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2">
+      <c r="H2">
+        <v>500</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>2018</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <f>TRUNC((C2&gt;9000)*(C2&lt;13996)*(997.8*(C2-9000)/10000+1400)*(C2-9000)/10000+(C2&gt;13996)*(C2&lt;54949)*((220.13*(C2-13996)/10000+2397)*(C2-13996)/10000+948.49)+(C2&gt;54950)*(C2&lt;260532)*(0.42*C2-8621.75)+(C2&gt;260532)*(0.45*C2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <f>TRUNC((D2&gt;9000)*(D2&lt;13996)*(997.8*(D2-9000)/10000+1400)*(D2-9000)/10000+(D2&gt;13996)*(D2&lt;54949)*((220.13*(D2-13996)/10000+2397)*(D2-13996)/10000+948.49)+(D2&gt;54950)*(D2&lt;260532)*(0.42*D2-8621.75)+(D2&gt;260532)*(0.45*D2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <f>TRUNC((E2&gt;9000)*(E2&lt;13996)*(997.8*(E2-9000)/10000+1400)*(E2-9000)/10000+(E2&gt;13996)*(E2&lt;54949)*((220.13*(E2-13996)/10000+2397)*(E2-13996)/10000+948.49)+(E2&gt;54950)*(E2&lt;260532)*(0.42*E2-8621.75)+(E2&gt;260532)*(0.45*E2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <f>TRUNC((F2&gt;9000)*(F2&lt;13996)*(997.8*(F2-9000)/10000+1400)*(F2-9000)/10000+(F2&gt;13996)*(F2&lt;54949)*((220.13*(F2-13996)/10000+2397)*(F2-13996)/10000+948.49)+(F2&gt;54950)*(F2&lt;260532)*(0.42*F2-8621.75)+(F2&gt;260532)*(0.45*F2-16437.7))</f>
         <v>0</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <f>MAX((G2-801)*0.25,0)</f>
         <v>0</v>
       </c>
-      <c r="P2">
-        <f>O2</f>
-        <v>0</v>
-      </c>
       <c r="Q2">
+        <f>P2</f>
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>9000</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>13996</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>54949</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>260532</v>
       </c>
-      <c r="Y2"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A6" si="0">B3</f>
         <v>2</v>
@@ -586,51 +595,54 @@
       <c r="G3">
         <v>2000</v>
       </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3">
+      <c r="H3">
+        <v>2000</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>2015</v>
       </c>
-      <c r="K3" s="2">
-        <f>TRUNC((C3&gt;Q3)*(C3&lt;R3)*(974.58*(C3-Q3)/10000+1400)*(C3-Q3)/10000+(C3&gt;R3)*(C3&lt;S3)*((228.74*(C3-R3)/10000+2397)*(C3-R3)/10000+971)+(C3&gt;S3)*(C3&lt;T3)*(0.42*C3-8239)+(C3&gt;T3)*(0.45*C3-15761))</f>
+      <c r="L3" s="2">
+        <f>TRUNC((C3&gt;R3)*(C3&lt;S3)*(974.58*(C3-R3)/10000+1400)*(C3-R3)/10000+(C3&gt;S3)*(C3&lt;T3)*((228.74*(C3-S3)/10000+2397)*(C3-S3)/10000+971)+(C3&gt;T3)*(C3&lt;U3)*(0.42*C3-8239)+(C3&gt;U3)*(0.45*C3-15761))</f>
         <v>236</v>
       </c>
-      <c r="L3" s="2">
-        <f>TRUNC((D3&gt;Q3)*(D3&lt;R3)*(974.58*(D3-Q3)/10000+1400)*(D3-Q3)/10000+(D3&gt;R3)*(D3&lt;S3)*((228.74*(D3-R3)/10000+2397)*(D3-R3)/10000+971)+(D3&gt;S3)*(D3&lt;T3)*(0.42*D3-8239)+(D3&gt;T3)*(0.45*D3-15761))</f>
+      <c r="M3" s="2">
+        <f>TRUNC((D3&gt;R3)*(D3&lt;S3)*(974.58*(D3-R3)/10000+1400)*(D3-R3)/10000+(D3&gt;S3)*(D3&lt;T3)*((228.74*(D3-S3)/10000+2397)*(D3-S3)/10000+971)+(D3&gt;T3)*(D3&lt;U3)*(0.42*D3-8239)+(D3&gt;U3)*(0.45*D3-15761))</f>
         <v>236</v>
       </c>
-      <c r="M3" s="2">
-        <f>TRUNC((E3&gt;Q3)*(E3&lt;R3)*(974.58*(E3-Q3)/10000+1400)*(E3-Q3)/10000+(E3&gt;R3)*(E3&lt;S3)*((228.74*(E3-R3)/10000+2397)*(E3-R3)/10000+971)+(E3&gt;S3)*(E3&lt;T3)*(0.42*E3-8239)+(E3&gt;T3)*(0.45*E3-15761))</f>
+      <c r="N3" s="2">
+        <f>TRUNC((E3&gt;R3)*(E3&lt;S3)*(974.58*(E3-R3)/10000+1400)*(E3-R3)/10000+(E3&gt;S3)*(E3&lt;T3)*((228.74*(E3-S3)/10000+2397)*(E3-S3)/10000+971)+(E3&gt;T3)*(E3&lt;U3)*(0.42*E3-8239)+(E3&gt;U3)*(0.45*E3-15761))</f>
         <v>615</v>
       </c>
-      <c r="N3" s="2">
-        <f>TRUNC((F3&gt;Q3)*(F3&lt;R3)*(974.58*(F3-Q3)/10000+1400)*(F3-Q3)/10000+(F3&gt;R3)*(F3&lt;T3)*((228.74*(F3-R3)/10000+2397)*(F3-S3)/10000+971)+(F3&gt;T3)*(F3&lt;T3)*(0.42*F3-8239)+(F3&gt;T3)*(0.45*F3-15761))</f>
+      <c r="O3" s="2">
+        <f>TRUNC((F3&gt;R3)*(F3&lt;S3)*(974.58*(F3-R3)/10000+1400)*(F3-R3)/10000+(F3&gt;S3)*(F3&lt;U3)*((228.74*(F3-S3)/10000+2397)*(F3-T3)/10000+971)+(F3&gt;U3)*(F3&lt;U3)*(0.42*F3-8239)+(F3&gt;U3)*(0.45*F3-15761))</f>
         <v>615</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O6" si="2">MAX((G3-801)*0.25,0)</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P6" si="2">MAX((G3-801)*0.25,0)</f>
         <v>299.75</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P6" si="3">O3</f>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q6" si="3">P3</f>
         <v>299.75</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>8472</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>13469</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>52881</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>250730</v>
       </c>
-      <c r="Y3"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -654,51 +666,54 @@
       <c r="G4">
         <v>1000</v>
       </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4">
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>2012</v>
       </c>
-      <c r="K4" s="2">
-        <f>TRUNC((C4&gt;Q4)*(C4&lt;R4)*(939.68*(C4-Q4)/10000+1400)*(C4-Q4)/10000+(C4&gt;R4)*(C4&lt;S4)*((228.74*(C4-R4)/10000+2397)*(C4-R4)/10000+1007)+(C4&gt;S4)*(C4&lt;T4)*(0.42*C4-8064)+(C4&gt;T4)*(0.45*C4-15576))</f>
+      <c r="L4" s="2">
+        <f>TRUNC((C4&gt;R4)*(C4&lt;S4)*(939.68*(C4-R4)/10000+1400)*(C4-R4)/10000+(C4&gt;S4)*(C4&lt;T4)*((228.74*(C4-S4)/10000+2397)*(C4-S4)/10000+1007)+(C4&gt;T4)*(C4&lt;U4)*(0.42*C4-8064)+(C4&gt;U4)*(0.45*C4-15576))</f>
         <v>2670</v>
       </c>
-      <c r="L4" s="2">
-        <f>TRUNC((D4&gt;Q4)*(D4&lt;R4)*(939.68*(D4-Q4)/10000+1400)*(D4-Q4)/10000+(D4&gt;R4)*(D4&lt;S4)*((228.74*(D4-R4)/10000+2397)*(D4-R4)/10000+1007)+(D4&gt;S4)*(D4&lt;T4)*(0.42*D4-8064)+(D4&gt;T4)*(0.45*D4-15576))</f>
+      <c r="M4" s="2">
+        <f>TRUNC((D4&gt;R4)*(D4&lt;S4)*(939.68*(D4-R4)/10000+1400)*(D4-R4)/10000+(D4&gt;S4)*(D4&lt;T4)*((228.74*(D4-S4)/10000+2397)*(D4-S4)/10000+1007)+(D4&gt;T4)*(D4&lt;U4)*(0.42*D4-8064)+(D4&gt;U4)*(0.45*D4-15576))</f>
         <v>2670</v>
       </c>
-      <c r="M4" s="2">
-        <f>TRUNC((E4&gt;Q4)*(E4&lt;R4)*(939.68*(E4-Q4)/10000+1400)*(E4-Q4)/10000+(E4&gt;R4)*(E4&lt;S4)*((228.74*(E4-R4)/10000+2397)*(E4-R4)/10000+1007)+(E4&gt;S4)*(E4&lt;T4)*(0.42*E4-8064)+(E4&gt;T4)*(0.45*E4-15576))</f>
+      <c r="N4" s="2">
+        <f>TRUNC((E4&gt;R4)*(E4&lt;S4)*(939.68*(E4-R4)/10000+1400)*(E4-R4)/10000+(E4&gt;S4)*(E4&lt;T4)*((228.74*(E4-S4)/10000+2397)*(E4-S4)/10000+1007)+(E4&gt;T4)*(E4&lt;U4)*(0.42*E4-8064)+(E4&gt;U4)*(0.45*E4-15576))</f>
         <v>2941</v>
       </c>
-      <c r="N4" s="2">
-        <f>TRUNC((F4&gt;Q4)*(F4&lt;R4)*(939.68*(F4-Q4)/10000+1400)*(F4-Q4)/10000+(F4&gt;R4)*(F4&lt;S4)*((228.74*(F4-R4)/10000+2397)*(F4-R4)/10000+1007)+(F4&gt;S4)*(F4&lt;T4)*(0.42*F4-8064)+(F4&gt;T4)*(0.45*F4-15576))</f>
+      <c r="O4" s="2">
+        <f>TRUNC((F4&gt;R4)*(F4&lt;S4)*(939.68*(F4-R4)/10000+1400)*(F4-R4)/10000+(F4&gt;S4)*(F4&lt;T4)*((228.74*(F4-S4)/10000+2397)*(F4-S4)/10000+1007)+(F4&gt;T4)*(F4&lt;U4)*(0.42*F4-8064)+(F4&gt;U4)*(0.45*F4-15576))</f>
         <v>2941</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f t="shared" si="2"/>
         <v>49.75</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f t="shared" si="3"/>
         <v>49.75</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>8004</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>13469</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>52881</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>250730</v>
       </c>
-      <c r="Y4"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -721,51 +736,54 @@
       <c r="G5">
         <v>2500</v>
       </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5">
+      <c r="H5">
+        <v>2500</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>2009</v>
       </c>
-      <c r="K5" s="2">
-        <f>TRUNC((C5&gt;Q5)*(C5&lt;R5)*(883.74*(C5-Q5)/10000+1500)*(C5-Q5)/10000+(C5&gt;R5)*(C5&lt;S5)*((228.74*(C5-R5)/10000+2397)*(C5-R5)/10000+989)+(C5&gt;S5)*(C5&lt;T5)*(0.42*C5-7914)+(C5&gt;T5)*(0.45*C5-15414))</f>
+      <c r="L5" s="2">
+        <f>TRUNC((C5&gt;R5)*(C5&lt;S5)*(883.74*(C5-R5)/10000+1500)*(C5-R5)/10000+(C5&gt;S5)*(C5&lt;T5)*((228.74*(C5-S5)/10000+2397)*(C5-S5)/10000+989)+(C5&gt;T5)*(C5&lt;U5)*(0.42*C5-7914)+(C5&gt;U5)*(0.45*C5-15414))</f>
         <v>13096</v>
       </c>
-      <c r="L5" s="2">
-        <f>TRUNC((D5&gt;Q5)*(D5&lt;R5)*(883.74*(D5-Q5)/10000+1500)*(D5-Q5)/10000+(D5&gt;R5)*(D5&lt;S5)*((228.74*(D5-R5)/10000+2397)*(D5-R5)/10000+989)+(D5&gt;S5)*(D5&lt;T5)*(0.42*D5-7914)+(D5&gt;T5)*(0.45*D5-15414))</f>
+      <c r="M5" s="2">
+        <f>TRUNC((D5&gt;R5)*(D5&lt;S5)*(883.74*(D5-R5)/10000+1500)*(D5-R5)/10000+(D5&gt;S5)*(D5&lt;T5)*((228.74*(D5-S5)/10000+2397)*(D5-S5)/10000+989)+(D5&gt;T5)*(D5&lt;U5)*(0.42*D5-7914)+(D5&gt;U5)*(0.45*D5-15414))</f>
         <v>9961</v>
       </c>
-      <c r="M5" s="2">
-        <f>TRUNC((E5&gt;Q5)*(E5&lt;R5)*(883.74*(E5-Q5)/10000+1500)*(E5-Q5)/10000+(E5&gt;R5)*(E5&lt;S5)*((228.74*(E5-R5)/10000+2397)*(E5-R5)/10000+989)+(E5&gt;S5)*(E5&lt;T5)*(0.42*E5-7914)+(E5&gt;T5)*(0.45*E5-15414))</f>
+      <c r="N5" s="2">
+        <f>TRUNC((E5&gt;R5)*(E5&lt;S5)*(883.74*(E5-R5)/10000+1500)*(E5-R5)/10000+(E5&gt;S5)*(E5&lt;T5)*((228.74*(E5-S5)/10000+2397)*(E5-S5)/10000+989)+(E5&gt;T5)*(E5&lt;U5)*(0.42*E5-7914)+(E5&gt;U5)*(0.45*E5-15414))</f>
         <v>14136</v>
       </c>
-      <c r="N5" s="2">
-        <f>TRUNC((F5&gt;Q5)*(F5&lt;R5)*(883.74*(F5-Q5)/10000+1500)*(F5-Q5)/10000+(F5&gt;R5)*(F5&lt;S5)*((228.74*(F5-R5)/10000+2397)*(F5-R5)/10000+989)+(F5&gt;S5)*(F5&lt;T5)*(0.42*F5-7914)+(F5&gt;T5)*(0.45*F5-15414))</f>
+      <c r="O5" s="2">
+        <f>TRUNC((F5&gt;R5)*(F5&lt;S5)*(883.74*(F5-R5)/10000+1500)*(F5-R5)/10000+(F5&gt;S5)*(F5&lt;T5)*((228.74*(F5-S5)/10000+2397)*(F5-S5)/10000+989)+(F5&gt;T5)*(F5&lt;U5)*(0.42*F5-7914)+(F5&gt;U5)*(0.45*F5-15414))</f>
         <v>10909</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f t="shared" si="2"/>
         <v>424.75</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f t="shared" si="3"/>
         <v>424.75</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>7664</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>12739</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>52152</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>250000</v>
       </c>
-      <c r="Y5"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -788,100 +806,103 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>2018</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <f>TRUNC((C6&gt;9000)*(C6&lt;13996)*(997.8*(C6-9000)/10000+1400)*(C6-9000)/10000+(C6&gt;13996)*(C6&lt;54949)*((220.13*(C6-13996)/10000+2397)*(C6-13996)/10000+948.49)+(C6&gt;54950)*(C6&lt;260532)*(0.42*C6-8621.75)+(C6&gt;260532)*(0.45*C6-16437.7))</f>
         <v>75378</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <f>TRUNC((D6&gt;9000)*(D6&lt;13996)*(997.8*(D6-9000)/10000+1400)*(D6-9000)/10000+(D6&gt;13996)*(D6&lt;54949)*((220.13*(D6-13996)/10000+2397)*(D6-13996)/10000+948.49)+(D6&gt;54950)*(D6&lt;260532)*(0.42*D6-8621.75)+(D6&gt;260532)*(0.45*D6-16437.7))</f>
         <v>66978</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <f>TRUNC((E6&gt;9000)*(E6&lt;13996)*(997.8*(E6-9000)/10000+1400)*(E6-9000)/10000+(E6&gt;13996)*(E6&lt;54949)*((220.13*(E6-13996)/10000+2397)*(E6-13996)/10000+948.49)+(E6&gt;54950)*(E6&lt;260532)*(0.42*E6-8621.75)+(E6&gt;260532)*(0.45*E6-16437.7))</f>
         <v>75378</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <f>TRUNC((F6&gt;9000)*(F6&lt;13996)*(997.8*(F6-9000)/10000+1400)*(F6-9000)/10000+(F6&gt;13996)*(F6&lt;54949)*((220.13*(F6-13996)/10000+2397)*(F6-13996)/10000+948.49)+(F6&gt;54950)*(F6&lt;260532)*(0.42*F6-8621.75)+(F6&gt;260532)*(0.45*F6-16437.7))</f>
         <v>66978</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>9000</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>13996</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>54949</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>260532</v>
       </c>
-      <c r="Y6"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y7" s="2"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y14" s="2"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y15" s="2"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="25:25" x14ac:dyDescent="0.25">
-      <c r="Y17" s="2"/>
-    </row>
-    <row r="18" spans="25:25" x14ac:dyDescent="0.25">
-      <c r="Y18" s="2"/>
-    </row>
-    <row r="19" spans="25:25" x14ac:dyDescent="0.25">
-      <c r="Y19" s="2"/>
-    </row>
-    <row r="20" spans="25:25" x14ac:dyDescent="0.25">
-      <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="25:25" x14ac:dyDescent="0.25">
-      <c r="Y21" s="2"/>
-    </row>
-    <row r="22" spans="25:25" x14ac:dyDescent="0.25">
-      <c r="Y22" s="2"/>
-    </row>
-    <row r="23" spans="25:25" x14ac:dyDescent="0.25">
-      <c r="Y23" s="2"/>
+      <c r="Z6"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z10" s="2"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z11" s="2"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z12" s="2"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z13" s="2"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z14" s="2"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z16" s="2"/>
+    </row>
+    <row r="17" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z17" s="2"/>
+    </row>
+    <row r="18" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z18" s="2"/>
+    </row>
+    <row r="19" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z19" s="2"/>
+    </row>
+    <row r="20" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z20" s="2"/>
+    </row>
+    <row r="21" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z21" s="2"/>
+    </row>
+    <row r="22" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z22" s="2"/>
+    </row>
+    <row r="23" spans="26:26" x14ac:dyDescent="0.25">
+      <c r="Z23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tax sched test correction #3
Former-commit-id: f2e824eacb52bcf446f7ae9f96147364ed0e92ae
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_tax_sched.xlsx
+++ b/tests/test_data/test_dfs_tax_sched.xlsx
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,19 +534,19 @@
         <v>2018</v>
       </c>
       <c r="L2" s="2">
-        <f>TRUNC((C2&gt;9000)*(C2&lt;13996)*(997.8*(C2-9000)/10000+1400)*(C2-9000)/10000+(C2&gt;13996)*(C2&lt;54949)*((220.13*(C2-13996)/10000+2397)*(C2-13996)/10000+948.49)+(C2&gt;54950)*(C2&lt;260532)*(0.42*C2-8621.75)+(C2&gt;260532)*(0.45*C2-16437.7))</f>
+        <f>(C2&gt;9000)*(C2&lt;13996)*(997.8*(C2-9000)/10000+1400)*(C2-9000)/10000+(C2&gt;13996)*(C2&lt;54949)*((220.13*(C2-13996)/10000+2397)*(C2-13996)/10000+948.49)+(C2&gt;54950)*(C2&lt;260532)*(0.42*C2-8621.75)+(C2&gt;260532)*(0.45*C2-16437.7)</f>
         <v>0</v>
       </c>
       <c r="M2" s="2">
-        <f>TRUNC((D2&gt;9000)*(D2&lt;13996)*(997.8*(D2-9000)/10000+1400)*(D2-9000)/10000+(D2&gt;13996)*(D2&lt;54949)*((220.13*(D2-13996)/10000+2397)*(D2-13996)/10000+948.49)+(D2&gt;54950)*(D2&lt;260532)*(0.42*D2-8621.75)+(D2&gt;260532)*(0.45*D2-16437.7))</f>
+        <f>(D2&gt;9000)*(D2&lt;13996)*(997.8*(D2-9000)/10000+1400)*(D2-9000)/10000+(D2&gt;13996)*(D2&lt;54949)*((220.13*(D2-13996)/10000+2397)*(D2-13996)/10000+948.49)+(D2&gt;54950)*(D2&lt;260532)*(0.42*D2-8621.75)+(D2&gt;260532)*(0.45*D2-16437.7)</f>
         <v>0</v>
       </c>
       <c r="N2" s="2">
-        <f>TRUNC((E2&gt;9000)*(E2&lt;13996)*(997.8*(E2-9000)/10000+1400)*(E2-9000)/10000+(E2&gt;13996)*(E2&lt;54949)*((220.13*(E2-13996)/10000+2397)*(E2-13996)/10000+948.49)+(E2&gt;54950)*(E2&lt;260532)*(0.42*E2-8621.75)+(E2&gt;260532)*(0.45*E2-16437.7))</f>
+        <f>(E2&gt;9000)*(E2&lt;13996)*(997.8*(E2-9000)/10000+1400)*(E2-9000)/10000+(E2&gt;13996)*(E2&lt;54949)*((220.13*(E2-13996)/10000+2397)*(E2-13996)/10000+948.49)+(E2&gt;54950)*(E2&lt;260532)*(0.42*E2-8621.75)+(E2&gt;260532)*(0.45*E2-16437.7)</f>
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <f>TRUNC((F2&gt;9000)*(F2&lt;13996)*(997.8*(F2-9000)/10000+1400)*(F2-9000)/10000+(F2&gt;13996)*(F2&lt;54949)*((220.13*(F2-13996)/10000+2397)*(F2-13996)/10000+948.49)+(F2&gt;54950)*(F2&lt;260532)*(0.42*F2-8621.75)+(F2&gt;260532)*(0.45*F2-16437.7))</f>
+        <f>(F2&gt;9000)*(F2&lt;13996)*(997.8*(F2-9000)/10000+1400)*(F2-9000)/10000+(F2&gt;13996)*(F2&lt;54949)*((220.13*(F2-13996)/10000+2397)*(F2-13996)/10000+948.49)+(F2&gt;54950)*(F2&lt;260532)*(0.42*F2-8621.75)+(F2&gt;260532)*(0.45*F2-16437.7)</f>
         <v>0</v>
       </c>
       <c r="P2">
@@ -605,20 +605,20 @@
         <v>2015</v>
       </c>
       <c r="L3" s="2">
-        <f>TRUNC((C3&gt;R3)*(C3&lt;S3)*(974.58*(C3-R3)/10000+1400)*(C3-R3)/10000+(C3&gt;S3)*(C3&lt;T3)*((228.74*(C3-S3)/10000+2397)*(C3-S3)/10000+971)+(C3&gt;T3)*(C3&lt;U3)*(0.42*C3-8239)+(C3&gt;U3)*(0.45*C3-15761))</f>
-        <v>236</v>
+        <f>(C3&gt;R3)*(C3&lt;S3)*(974.58*(C3-R3)/10000+1400)*(C3-R3)/10000+(C3&gt;S3)*(C3&lt;T3)*((228.74*(C3-S3)/10000+2397)*(C3-S3)/10000+971)+(C3&gt;T3)*(C3&lt;U3)*(0.42*C3-8239)+(C3&gt;U3)*(0.45*C3-15761)</f>
+        <v>236.67433790719997</v>
       </c>
       <c r="M3" s="2">
-        <f>TRUNC((D3&gt;R3)*(D3&lt;S3)*(974.58*(D3-R3)/10000+1400)*(D3-R3)/10000+(D3&gt;S3)*(D3&lt;T3)*((228.74*(D3-S3)/10000+2397)*(D3-S3)/10000+971)+(D3&gt;T3)*(D3&lt;U3)*(0.42*D3-8239)+(D3&gt;U3)*(0.45*D3-15761))</f>
-        <v>236</v>
+        <f>(D3&gt;R3)*(D3&lt;S3)*(974.58*(D3-R3)/10000+1400)*(D3-R3)/10000+(D3&gt;S3)*(D3&lt;T3)*((228.74*(D3-S3)/10000+2397)*(D3-S3)/10000+971)+(D3&gt;T3)*(D3&lt;U3)*(0.42*D3-8239)+(D3&gt;U3)*(0.45*D3-15761)</f>
+        <v>236.67433790719997</v>
       </c>
       <c r="N3" s="2">
-        <f>TRUNC((E3&gt;R3)*(E3&lt;S3)*(974.58*(E3-R3)/10000+1400)*(E3-R3)/10000+(E3&gt;S3)*(E3&lt;T3)*((228.74*(E3-S3)/10000+2397)*(E3-S3)/10000+971)+(E3&gt;T3)*(E3&lt;U3)*(0.42*E3-8239)+(E3&gt;U3)*(0.45*E3-15761))</f>
-        <v>615</v>
+        <f>(E3&gt;R3)*(E3&lt;S3)*(974.58*(E3-R3)/10000+1400)*(E3-R3)/10000+(E3&gt;S3)*(E3&lt;T3)*((228.74*(E3-S3)/10000+2397)*(E3-S3)/10000+971)+(E3&gt;T3)*(E3&lt;U3)*(0.42*E3-8239)+(E3&gt;U3)*(0.45*E3-15761)</f>
+        <v>615.2238675072</v>
       </c>
       <c r="O3" s="2">
-        <f>TRUNC((F3&gt;R3)*(F3&lt;S3)*(974.58*(F3-R3)/10000+1400)*(F3-R3)/10000+(F3&gt;S3)*(F3&lt;U3)*((228.74*(F3-S3)/10000+2397)*(F3-T3)/10000+971)+(F3&gt;U3)*(F3&lt;U3)*(0.42*F3-8239)+(F3&gt;U3)*(0.45*F3-15761))</f>
-        <v>615</v>
+        <f>(F3&gt;R3)*(F3&lt;S3)*(974.58*(F3-R3)/10000+1400)*(F3-R3)/10000+(F3&gt;S3)*(F3&lt;U3)*((228.74*(F3-S3)/10000+2397)*(F3-T3)/10000+971)+(F3&gt;U3)*(F3&lt;U3)*(0.42*F3-8239)+(F3&gt;U3)*(0.45*F3-15761)</f>
+        <v>615.2238675072</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P6" si="2">MAX((G3-801)*0.25,0)</f>
@@ -676,20 +676,20 @@
         <v>2012</v>
       </c>
       <c r="L4" s="2">
-        <f>TRUNC((C4&gt;R4)*(C4&lt;S4)*(939.68*(C4-R4)/10000+1400)*(C4-R4)/10000+(C4&gt;S4)*(C4&lt;T4)*((228.74*(C4-S4)/10000+2397)*(C4-S4)/10000+1007)+(C4&gt;T4)*(C4&lt;U4)*(0.42*C4-8064)+(C4&gt;U4)*(0.45*C4-15576))</f>
-        <v>2670</v>
+        <f>(C4&gt;R4)*(C4&lt;S4)*(912.17*(C4-R4)/10000+1400)*(C4-R4)/10000+(C4&gt;S4)*(C4&lt;T4)*((228.74*(C4-S4)/10000+2397)*(C4-S4)/10000+1038)+(C4&gt;T4)*(C4&lt;U4)*(0.42*C4-8172)+(C4&gt;U4)*(0.45*C4-15694)</f>
+        <v>2700.7777946599999</v>
       </c>
       <c r="M4" s="2">
-        <f>TRUNC((D4&gt;R4)*(D4&lt;S4)*(939.68*(D4-R4)/10000+1400)*(D4-R4)/10000+(D4&gt;S4)*(D4&lt;T4)*((228.74*(D4-S4)/10000+2397)*(D4-S4)/10000+1007)+(D4&gt;T4)*(D4&lt;U4)*(0.42*D4-8064)+(D4&gt;U4)*(0.45*D4-15576))</f>
-        <v>2670</v>
+        <f>(D4&gt;R4)*(D4&lt;S4)*(912.17*(D4-R4)/10000+1400)*(D4-R4)/10000+(D4&gt;S4)*(D4&lt;T4)*((228.74*(D4-S4)/10000+2397)*(D4-S4)/10000+1038)+(D4&gt;T4)*(D4&lt;U4)*(0.42*D4-8172)+(D4&gt;U4)*(0.45*D4-15694)</f>
+        <v>2700.7777946599999</v>
       </c>
       <c r="N4" s="2">
-        <f>TRUNC((E4&gt;R4)*(E4&lt;S4)*(939.68*(E4-R4)/10000+1400)*(E4-R4)/10000+(E4&gt;S4)*(E4&lt;T4)*((228.74*(E4-S4)/10000+2397)*(E4-S4)/10000+1007)+(E4&gt;T4)*(E4&lt;U4)*(0.42*E4-8064)+(E4&gt;U4)*(0.45*E4-15576))</f>
-        <v>2941</v>
+        <f>(E4&gt;R4)*(E4&lt;S4)*(912.17*(E4-R4)/10000+1400)*(E4-R4)/10000+(E4&gt;S4)*(E4&lt;T4)*((228.74*(E4-S4)/10000+2397)*(E4-S4)/10000+1038)+(E4&gt;T4)*(E4&lt;U4)*(0.42*E4-8172)+(E4&gt;U4)*(0.45*E4-15694)</f>
+        <v>2972.6386386599997</v>
       </c>
       <c r="O4" s="2">
-        <f>TRUNC((F4&gt;R4)*(F4&lt;S4)*(939.68*(F4-R4)/10000+1400)*(F4-R4)/10000+(F4&gt;S4)*(F4&lt;T4)*((228.74*(F4-S4)/10000+2397)*(F4-S4)/10000+1007)+(F4&gt;T4)*(F4&lt;U4)*(0.42*F4-8064)+(F4&gt;U4)*(0.45*F4-15576))</f>
-        <v>2941</v>
+        <f>(F4&gt;R4)*(F4&lt;S4)*(912.17*(F4-R4)/10000+1400)*(F4-R4)/10000+(F4&gt;S4)*(F4&lt;T4)*((228.74*(F4-S4)/10000+2397)*(F4-S4)/10000+1038)+(F4&gt;T4)*(F4&lt;U4)*(0.42*F4-8172)+(F4&gt;U4)*(0.45*F4-15694)</f>
+        <v>2972.6386386599997</v>
       </c>
       <c r="P4">
         <f t="shared" si="2"/>
@@ -700,10 +700,10 @@
         <v>49.75</v>
       </c>
       <c r="R4">
-        <v>8004</v>
+        <v>8005</v>
       </c>
       <c r="S4">
-        <v>13469</v>
+        <v>13470</v>
       </c>
       <c r="T4">
         <v>52881</v>
@@ -746,20 +746,20 @@
         <v>2009</v>
       </c>
       <c r="L5" s="2">
-        <f>TRUNC((C5&gt;R5)*(C5&lt;S5)*(883.74*(C5-R5)/10000+1500)*(C5-R5)/10000+(C5&gt;S5)*(C5&lt;T5)*((228.74*(C5-S5)/10000+2397)*(C5-S5)/10000+989)+(C5&gt;T5)*(C5&lt;U5)*(0.42*C5-7914)+(C5&gt;U5)*(0.45*C5-15414))</f>
-        <v>13096</v>
+        <f>(C5&gt;R5)*(C5&lt;S5)*(883.74*(C5-R5)/10000+1500)*(C5-R5)/10000+(C5&gt;S5)*(C5&lt;T5)*((228.74*(C5-S5)/10000+2397)*(C5-S5)/10000+989)+(C5&gt;T5)*(C5&lt;U5)*(0.42*C5-7914)+(C5&gt;U5)*(0.45*C5-15414)</f>
+        <v>13096.246963575401</v>
       </c>
       <c r="M5" s="2">
-        <f>TRUNC((D5&gt;R5)*(D5&lt;S5)*(883.74*(D5-R5)/10000+1500)*(D5-R5)/10000+(D5&gt;S5)*(D5&lt;T5)*((228.74*(D5-S5)/10000+2397)*(D5-S5)/10000+989)+(D5&gt;T5)*(D5&lt;U5)*(0.42*D5-7914)+(D5&gt;U5)*(0.45*D5-15414))</f>
-        <v>9961</v>
+        <f>(D5&gt;R5)*(D5&lt;S5)*(883.74*(D5-R5)/10000+1500)*(D5-R5)/10000+(D5&gt;S5)*(D5&lt;T5)*((228.74*(D5-S5)/10000+2397)*(D5-S5)/10000+989)+(D5&gt;T5)*(D5&lt;U5)*(0.42*D5-7914)+(D5&gt;U5)*(0.45*D5-15414)</f>
+        <v>9961.3475811753997</v>
       </c>
       <c r="N5" s="2">
-        <f>TRUNC((E5&gt;R5)*(E5&lt;S5)*(883.74*(E5-R5)/10000+1500)*(E5-R5)/10000+(E5&gt;S5)*(E5&lt;T5)*((228.74*(E5-S5)/10000+2397)*(E5-S5)/10000+989)+(E5&gt;T5)*(E5&lt;U5)*(0.42*E5-7914)+(E5&gt;U5)*(0.45*E5-15414))</f>
+        <f>(E5&gt;R5)*(E5&lt;S5)*(883.74*(E5-R5)/10000+1500)*(E5-R5)/10000+(E5&gt;S5)*(E5&lt;T5)*((228.74*(E5-S5)/10000+2397)*(E5-S5)/10000+989)+(E5&gt;T5)*(E5&lt;U5)*(0.42*E5-7914)+(E5&gt;U5)*(0.45*E5-15414)</f>
         <v>14136</v>
       </c>
       <c r="O5" s="2">
-        <f>TRUNC((F5&gt;R5)*(F5&lt;S5)*(883.74*(F5-R5)/10000+1500)*(F5-R5)/10000+(F5&gt;S5)*(F5&lt;T5)*((228.74*(F5-S5)/10000+2397)*(F5-S5)/10000+989)+(F5&gt;T5)*(F5&lt;U5)*(0.42*F5-7914)+(F5&gt;U5)*(0.45*F5-15414))</f>
-        <v>10909</v>
+        <f>(F5&gt;R5)*(F5&lt;S5)*(883.74*(F5-R5)/10000+1500)*(F5-R5)/10000+(F5&gt;S5)*(F5&lt;T5)*((228.74*(F5-S5)/10000+2397)*(F5-S5)/10000+989)+(F5&gt;T5)*(F5&lt;U5)*(0.42*F5-7914)+(F5&gt;U5)*(0.45*F5-15414)</f>
+        <v>10909.551888175401</v>
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
@@ -816,20 +816,20 @@
         <v>2018</v>
       </c>
       <c r="L6" s="2">
-        <f>TRUNC((C6&gt;9000)*(C6&lt;13996)*(997.8*(C6-9000)/10000+1400)*(C6-9000)/10000+(C6&gt;13996)*(C6&lt;54949)*((220.13*(C6-13996)/10000+2397)*(C6-13996)/10000+948.49)+(C6&gt;54950)*(C6&lt;260532)*(0.42*C6-8621.75)+(C6&gt;260532)*(0.45*C6-16437.7))</f>
-        <v>75378</v>
+        <f>(C6&gt;9000)*(C6&lt;13996)*(997.8*(C6-9000)/10000+1400)*(C6-9000)/10000+(C6&gt;13996)*(C6&lt;54949)*((220.13*(C6-13996)/10000+2397)*(C6-13996)/10000+948.49)+(C6&gt;54950)*(C6&lt;260532)*(0.42*C6-8621.75)+(C6&gt;260532)*(0.45*C6-16437.7)</f>
+        <v>75378.25</v>
       </c>
       <c r="M6" s="2">
-        <f>TRUNC((D6&gt;9000)*(D6&lt;13996)*(997.8*(D6-9000)/10000+1400)*(D6-9000)/10000+(D6&gt;13996)*(D6&lt;54949)*((220.13*(D6-13996)/10000+2397)*(D6-13996)/10000+948.49)+(D6&gt;54950)*(D6&lt;260532)*(0.42*D6-8621.75)+(D6&gt;260532)*(0.45*D6-16437.7))</f>
-        <v>66978</v>
+        <f>(D6&gt;9000)*(D6&lt;13996)*(997.8*(D6-9000)/10000+1400)*(D6-9000)/10000+(D6&gt;13996)*(D6&lt;54949)*((220.13*(D6-13996)/10000+2397)*(D6-13996)/10000+948.49)+(D6&gt;54950)*(D6&lt;260532)*(0.42*D6-8621.75)+(D6&gt;260532)*(0.45*D6-16437.7)</f>
+        <v>66978.25</v>
       </c>
       <c r="N6" s="2">
-        <f>TRUNC((E6&gt;9000)*(E6&lt;13996)*(997.8*(E6-9000)/10000+1400)*(E6-9000)/10000+(E6&gt;13996)*(E6&lt;54949)*((220.13*(E6-13996)/10000+2397)*(E6-13996)/10000+948.49)+(E6&gt;54950)*(E6&lt;260532)*(0.42*E6-8621.75)+(E6&gt;260532)*(0.45*E6-16437.7))</f>
-        <v>75378</v>
+        <f>(E6&gt;9000)*(E6&lt;13996)*(997.8*(E6-9000)/10000+1400)*(E6-9000)/10000+(E6&gt;13996)*(E6&lt;54949)*((220.13*(E6-13996)/10000+2397)*(E6-13996)/10000+948.49)+(E6&gt;54950)*(E6&lt;260532)*(0.42*E6-8621.75)+(E6&gt;260532)*(0.45*E6-16437.7)</f>
+        <v>75378.25</v>
       </c>
       <c r="O6" s="2">
-        <f>TRUNC((F6&gt;9000)*(F6&lt;13996)*(997.8*(F6-9000)/10000+1400)*(F6-9000)/10000+(F6&gt;13996)*(F6&lt;54949)*((220.13*(F6-13996)/10000+2397)*(F6-13996)/10000+948.49)+(F6&gt;54950)*(F6&lt;260532)*(0.42*F6-8621.75)+(F6&gt;260532)*(0.45*F6-16437.7))</f>
-        <v>66978</v>
+        <f>(F6&gt;9000)*(F6&lt;13996)*(997.8*(F6-9000)/10000+1400)*(F6-9000)/10000+(F6&gt;13996)*(F6&lt;54949)*((220.13*(F6-13996)/10000+2397)*(F6-13996)/10000+948.49)+(F6&gt;54950)*(F6&lt;260532)*(0.42*F6-8621.75)+(F6&gt;260532)*(0.45*F6-16437.7)</f>
+        <v>66978.25</v>
       </c>
       <c r="P6">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
tax sched correction #4
Former-commit-id: dabf9eef2240477ba8858e007a66b6c1cf7a9070
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_tax_sched.xlsx
+++ b/tests/test_data/test_dfs_tax_sched.xlsx
@@ -426,7 +426,7 @@
   <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="L3" sqref="L3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,20 +605,20 @@
         <v>2015</v>
       </c>
       <c r="L3" s="2">
-        <f>(C3&gt;R3)*(C3&lt;S3)*(974.58*(C3-R3)/10000+1400)*(C3-R3)/10000+(C3&gt;S3)*(C3&lt;T3)*((228.74*(C3-S3)/10000+2397)*(C3-S3)/10000+971)+(C3&gt;T3)*(C3&lt;U3)*(0.42*C3-8239)+(C3&gt;U3)*(0.45*C3-15761)</f>
-        <v>236.67433790719997</v>
+        <f>(C3&gt;R3)*(C3&lt;S3)*((997.6*(C3-R3)/10000+1400)*(C3-R3)/10000)+(C3&gt;S3)*(C3&lt;T3)*((228.74*(C3-S3)/10000+2397)*(C3-S3)/10000+971)+(C3&gt;T3)*(C3&lt;U3)*(0.42*C3-8239)+(C3&gt;U3)*(0.45*C3-15761)</f>
+        <v>237.21180518399999</v>
       </c>
       <c r="M3" s="2">
-        <f>(D3&gt;R3)*(D3&lt;S3)*(974.58*(D3-R3)/10000+1400)*(D3-R3)/10000+(D3&gt;S3)*(D3&lt;T3)*((228.74*(D3-S3)/10000+2397)*(D3-S3)/10000+971)+(D3&gt;T3)*(D3&lt;U3)*(0.42*D3-8239)+(D3&gt;U3)*(0.45*D3-15761)</f>
-        <v>236.67433790719997</v>
+        <f>(D3&gt;R3)*(D3&lt;S3)*(997.6*(D3-R3)/10000+1400)*(D3-R3)/10000+(D3&gt;S3)*(D3&lt;T3)*((228.74*(D3-S3)/10000+2397)*(D3-S3)/10000+971)+(D3&gt;T3)*(D3&lt;U3)*(0.42*D3-8239)+(D3&gt;U3)*(0.45*D3-15761)</f>
+        <v>237.21180518399999</v>
       </c>
       <c r="N3" s="2">
-        <f>(E3&gt;R3)*(E3&lt;S3)*(974.58*(E3-R3)/10000+1400)*(E3-R3)/10000+(E3&gt;S3)*(E3&lt;T3)*((228.74*(E3-S3)/10000+2397)*(E3-S3)/10000+971)+(E3&gt;T3)*(E3&lt;U3)*(0.42*E3-8239)+(E3&gt;U3)*(0.45*E3-15761)</f>
-        <v>615.2238675072</v>
+        <f>(E3&gt;R3)*(E3&lt;S3)*(997.6*(E3-R3)/10000+1400)*(E3-R3)/10000+(E3&gt;S3)*(E3&lt;T3)*((228.74*(E3-S3)/10000+2397)*(E3-S3)/10000+971)+(E3&gt;T3)*(E3&lt;U3)*(0.42*E3-8239)+(E3&gt;U3)*(0.45*E3-15761)</f>
+        <v>618.08911718399997</v>
       </c>
       <c r="O3" s="2">
-        <f>(F3&gt;R3)*(F3&lt;S3)*(974.58*(F3-R3)/10000+1400)*(F3-R3)/10000+(F3&gt;S3)*(F3&lt;U3)*((228.74*(F3-S3)/10000+2397)*(F3-T3)/10000+971)+(F3&gt;U3)*(F3&lt;U3)*(0.42*F3-8239)+(F3&gt;U3)*(0.45*F3-15761)</f>
-        <v>615.2238675072</v>
+        <f>(F3&gt;R3)*(F3&lt;S3)*(997.6*(F3-R3)/10000+1400)*(F3-R3)/10000+(F3&gt;S3)*(F3&lt;U3)*((228.74*(F3-S3)/10000+2397)*(F3-T3)/10000+971)+(F3&gt;U3)*(F3&lt;U3)*(0.42*F3-8239)+(F3&gt;U3)*(0.45*F3-15761)</f>
+        <v>618.08911718399997</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P6" si="2">MAX((G3-801)*0.25,0)</f>

</xml_diff>